<commit_message>
Aggiunti valori non misurabili per bf1 su 940MX e GTX1070
</commit_message>
<xml_diff>
--- a/performance bf1.xlsx
+++ b/performance bf1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B877B8C-1F7F-4812-99F7-B4FABA1D2BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D780041-7A07-463B-A113-BF7FEED43CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="26">
   <si>
     <t>SPEEDUP</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>bf1-soa-sh</t>
+  </si>
+  <si>
+    <t>&gt;1h</t>
+  </si>
+  <si>
+    <t>THROUGHPUT</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -310,10 +319,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:AO83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="AD37" sqref="AD37:AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,45 +618,81 @@
     <col min="3" max="20" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-    </row>
-    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="V1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+    </row>
+    <row r="3" spans="1:41" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -702,8 +747,65 @@
       <c r="T4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="15"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -737,13 +839,49 @@
         <f>AVERAGE(O5:S5)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="15"/>
+      <c r="V5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="5" t="e">
+        <f>AVERAGE(X5:AB5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="5" t="e">
+        <f>AVERAGE(AD5:AH5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="5" t="e">
+        <f>AVERAGE(AJ5:AN5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -752,14 +890,16 @@
         <f t="shared" ref="H6:H13" si="0">AVERAGE(C6:G6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9">
+        <v>2631.8240000000001</v>
+      </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="11"/>
-      <c r="N6" s="5" t="e">
+      <c r="N6" s="5">
         <f t="shared" ref="N6:N13" si="1">AVERAGE(I6:M6)</f>
-        <v>#DIV/0!</v>
+        <v>2631.8240000000001</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="10"/>
@@ -770,13 +910,59 @@
         <f t="shared" ref="T6:T13" si="2">AVERAGE(O6:S6)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="15"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC6" s="5" t="e">
+        <f t="shared" ref="AC6:AC13" si="3">AVERAGE(X6:AB6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>2.234</v>
+      </c>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="5">
+        <f t="shared" ref="AI6:AI13" si="4">AVERAGE(AD6:AH6)</f>
+        <v>2.234</v>
+      </c>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="5" t="e">
+        <f t="shared" ref="AO6:AO13" si="5">AVERAGE(AJ6:AN6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -785,7 +971,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -803,13 +991,67 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="15"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC7" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI7" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -818,7 +1060,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
@@ -836,13 +1080,67 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="15"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC8" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI8" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -851,7 +1149,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -869,8 +1169,60 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="15"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC9" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI9" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
@@ -902,8 +1254,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="15"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -935,8 +1319,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="15"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
@@ -968,8 +1384,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="15"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="10"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -1001,8 +1449,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="15"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ13" s="12"/>
+      <c r="AK13" s="13"/>
+      <c r="AL13" s="13"/>
+      <c r="AM13" s="13"/>
+      <c r="AN13" s="14"/>
+      <c r="AO13" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="16"/>
       <c r="C14" s="15"/>
@@ -1023,8 +1503,29 @@
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="15"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="15"/>
+      <c r="AO14" s="15"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>20</v>
       </c>
@@ -1058,29 +1559,67 @@
         <f>AVERAGE(O15:S15)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="15"/>
+      <c r="V15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="5" t="e">
+        <f>AVERAGE(X15:AB15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="8"/>
+      <c r="AI15" s="5" t="e">
+        <f>AVERAGE(AD15:AH15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+      <c r="AN15" s="8"/>
+      <c r="AO15" s="5" t="e">
+        <f>AVERAGE(AJ15:AN15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9">
+        <v>3204.047</v>
+      </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="5" t="e">
-        <f t="shared" ref="H16:H23" si="3">AVERAGE(C16:G16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="9"/>
+      <c r="H16" s="5">
+        <f t="shared" ref="H16:H23" si="6">AVERAGE(C16:G16)</f>
+        <v>3204.047</v>
+      </c>
+      <c r="I16" s="9">
+        <v>2186.4749999999999</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="5" t="e">
-        <f t="shared" ref="N16:N23" si="4">AVERAGE(I16:M16)</f>
-        <v>#DIV/0!</v>
+      <c r="N16" s="5">
+        <f t="shared" ref="N16:N23" si="7">AVERAGE(I16:M16)</f>
+        <v>2186.4749999999999</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="10"/>
@@ -1088,31 +1627,69 @@
       <c r="R16" s="10"/>
       <c r="S16" s="11"/>
       <c r="T16" s="5" t="e">
-        <f t="shared" ref="T16:T23" si="5">AVERAGE(O16:S16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T16:T23" si="8">AVERAGE(O16:S16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" s="15"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="5" t="e">
+        <f t="shared" ref="AC16:AC23" si="9">AVERAGE(X16:AB16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>2.6909999999999998</v>
+      </c>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="5">
+        <f t="shared" ref="AI16:AI23" si="10">AVERAGE(AD16:AH16)</f>
+        <v>2.6909999999999998</v>
+      </c>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="10"/>
+      <c r="AL16" s="10"/>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="5" t="e">
+        <f t="shared" ref="AO16:AO23" si="11">AVERAGE(AJ16:AN16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
       <c r="H17" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="9"/>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="11"/>
       <c r="N17" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O17" s="9"/>
@@ -1121,31 +1698,87 @@
       <c r="R17" s="10"/>
       <c r="S17" s="11"/>
       <c r="T17" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U17" s="15"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC17" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI17" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11"/>
       <c r="H18" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="9"/>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="11"/>
       <c r="N18" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="9"/>
@@ -1154,31 +1787,87 @@
       <c r="R18" s="10"/>
       <c r="S18" s="11"/>
       <c r="T18" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U18" s="15"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC18" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI18" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="10"/>
+      <c r="AM18" s="10"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="9"/>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="11"/>
       <c r="N19" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O19" s="9"/>
@@ -1187,11 +1876,63 @@
       <c r="R19" s="10"/>
       <c r="S19" s="11"/>
       <c r="T19" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U19" s="15"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC19" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI19" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
@@ -1202,7 +1943,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
       <c r="H20" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" s="9"/>
@@ -1211,7 +1952,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="11"/>
       <c r="N20" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O20" s="9"/>
@@ -1220,11 +1961,43 @@
       <c r="R20" s="10"/>
       <c r="S20" s="11"/>
       <c r="T20" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U20" s="15"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
@@ -1235,7 +2008,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I21" s="9"/>
@@ -1244,7 +2017,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="11"/>
       <c r="N21" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O21" s="9"/>
@@ -1253,11 +2026,43 @@
       <c r="R21" s="10"/>
       <c r="S21" s="11"/>
       <c r="T21" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="15"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="4" t="s">
         <v>8</v>
@@ -1268,7 +2073,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="H22" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" s="9"/>
@@ -1277,7 +2082,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="11"/>
       <c r="N22" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O22" s="9"/>
@@ -1286,11 +2091,43 @@
       <c r="R22" s="10"/>
       <c r="S22" s="11"/>
       <c r="T22" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" s="15"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="10"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="4" t="s">
         <v>9</v>
@@ -1301,7 +2138,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="14"/>
       <c r="H23" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I23" s="12"/>
@@ -1310,7 +2147,7 @@
       <c r="L23" s="13"/>
       <c r="M23" s="14"/>
       <c r="N23" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O23" s="12"/>
@@ -1319,11 +2156,43 @@
       <c r="R23" s="13"/>
       <c r="S23" s="14"/>
       <c r="T23" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" s="15"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD23" s="12"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ23" s="12"/>
+      <c r="AK23" s="13"/>
+      <c r="AL23" s="13"/>
+      <c r="AM23" s="13"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="16"/>
       <c r="C24" s="15"/>
@@ -1344,8 +2213,29 @@
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="15"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>21</v>
       </c>
@@ -1379,29 +2269,67 @@
         <f>AVERAGE(O25:S25)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25" s="15"/>
+      <c r="V25" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="W25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="5" t="e">
+        <f>AVERAGE(X25:AB25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="8"/>
+      <c r="AI25" s="5" t="e">
+        <f>AVERAGE(AD25:AH25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="7"/>
+      <c r="AL25" s="7"/>
+      <c r="AM25" s="7"/>
+      <c r="AN25" s="8"/>
+      <c r="AO25" s="5" t="e">
+        <f>AVERAGE(AJ25:AN25)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9">
+        <v>2645.5079999999998</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="11"/>
-      <c r="H26" s="5" t="e">
-        <f t="shared" ref="H26:H33" si="6">AVERAGE(C26:G26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" s="9"/>
+      <c r="H26" s="5">
+        <f t="shared" ref="H26:H33" si="12">AVERAGE(C26:G26)</f>
+        <v>2645.5079999999998</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1692.23</v>
+      </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="11"/>
-      <c r="N26" s="5" t="e">
-        <f t="shared" ref="N26:N33" si="7">AVERAGE(I26:M26)</f>
-        <v>#DIV/0!</v>
+      <c r="N26" s="5">
+        <f t="shared" ref="N26:N33" si="13">AVERAGE(I26:M26)</f>
+        <v>1692.23</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="10"/>
@@ -1409,31 +2337,71 @@
       <c r="R26" s="10"/>
       <c r="S26" s="11"/>
       <c r="T26" s="5" t="e">
-        <f t="shared" ref="T26:T33" si="8">AVERAGE(O26:S26)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T26:T33" si="14">AVERAGE(O26:S26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U26" s="15"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="9">
+        <v>2.2229999999999999</v>
+      </c>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="5">
+        <f t="shared" ref="AC26:AC33" si="15">AVERAGE(X26:AB26)</f>
+        <v>2.2229999999999999</v>
+      </c>
+      <c r="AD26" s="9">
+        <v>3.4750000000000001</v>
+      </c>
+      <c r="AE26" s="10"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="5">
+        <f t="shared" ref="AI26:AI33" si="16">AVERAGE(AD26:AH26)</f>
+        <v>3.4750000000000001</v>
+      </c>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="10"/>
+      <c r="AL26" s="10"/>
+      <c r="AM26" s="10"/>
+      <c r="AN26" s="11"/>
+      <c r="AO26" s="5" t="e">
+        <f t="shared" ref="AO26:AO33" si="17">AVERAGE(AJ26:AN26)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
       <c r="H27" s="5" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" s="9"/>
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="11"/>
       <c r="N27" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O27" s="9"/>
@@ -1442,31 +2410,87 @@
       <c r="R27" s="10"/>
       <c r="S27" s="11"/>
       <c r="T27" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U27" s="15"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC27" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI27" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="10"/>
+      <c r="AM27" s="10"/>
+      <c r="AN27" s="11"/>
+      <c r="AO27" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="11"/>
       <c r="H28" s="5" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="9"/>
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="11"/>
       <c r="N28" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O28" s="9"/>
@@ -1475,31 +2499,87 @@
       <c r="R28" s="10"/>
       <c r="S28" s="11"/>
       <c r="T28" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U28" s="15"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC28" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI28" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="10"/>
+      <c r="AL28" s="10"/>
+      <c r="AM28" s="10"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
       <c r="H29" s="5" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" s="9"/>
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="11"/>
       <c r="N29" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O29" s="9"/>
@@ -1508,11 +2588,63 @@
       <c r="R29" s="10"/>
       <c r="S29" s="11"/>
       <c r="T29" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U29" s="15"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC29" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI29" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ29" s="9"/>
+      <c r="AK29" s="10"/>
+      <c r="AL29" s="10"/>
+      <c r="AM29" s="10"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4" t="s">
         <v>6</v>
@@ -1523,7 +2655,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
       <c r="H30" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I30" s="9"/>
@@ -1532,7 +2664,7 @@
       <c r="L30" s="10"/>
       <c r="M30" s="11"/>
       <c r="N30" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O30" s="9"/>
@@ -1541,11 +2673,43 @@
       <c r="R30" s="10"/>
       <c r="S30" s="11"/>
       <c r="T30" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U30" s="15"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ30" s="9"/>
+      <c r="AK30" s="10"/>
+      <c r="AL30" s="10"/>
+      <c r="AM30" s="10"/>
+      <c r="AN30" s="11"/>
+      <c r="AO30" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
@@ -1556,7 +2720,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
       <c r="H31" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I31" s="9"/>
@@ -1565,7 +2729,7 @@
       <c r="L31" s="10"/>
       <c r="M31" s="11"/>
       <c r="N31" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O31" s="9"/>
@@ -1574,11 +2738,43 @@
       <c r="R31" s="10"/>
       <c r="S31" s="11"/>
       <c r="T31" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U31" s="15"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="10"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="10"/>
+      <c r="AL31" s="10"/>
+      <c r="AM31" s="10"/>
+      <c r="AN31" s="11"/>
+      <c r="AO31" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
@@ -1589,7 +2785,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
       <c r="H32" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I32" s="9"/>
@@ -1598,7 +2794,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="11"/>
       <c r="N32" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O32" s="9"/>
@@ -1607,11 +2803,43 @@
       <c r="R32" s="10"/>
       <c r="S32" s="11"/>
       <c r="T32" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U32" s="15"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="10"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="10"/>
+      <c r="AL32" s="10"/>
+      <c r="AM32" s="10"/>
+      <c r="AN32" s="11"/>
+      <c r="AO32" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4" t="s">
         <v>9</v>
@@ -1622,7 +2850,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
       <c r="H33" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I33" s="12"/>
@@ -1631,7 +2859,7 @@
       <c r="L33" s="13"/>
       <c r="M33" s="14"/>
       <c r="N33" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O33" s="12"/>
@@ -1640,11 +2868,43 @@
       <c r="R33" s="13"/>
       <c r="S33" s="14"/>
       <c r="T33" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U33" s="15"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="14"/>
+      <c r="AC33" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="13"/>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="13"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="13"/>
+      <c r="AL33" s="13"/>
+      <c r="AM33" s="13"/>
+      <c r="AN33" s="14"/>
+      <c r="AO33" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="16"/>
       <c r="C34" s="15"/>
@@ -1665,8 +2925,29 @@
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34" s="15"/>
+      <c r="V34" s="18"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
+      <c r="AC34" s="15"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="15"/>
+      <c r="AG34" s="15"/>
+      <c r="AH34" s="15"/>
+      <c r="AI34" s="15"/>
+      <c r="AJ34" s="15"/>
+      <c r="AK34" s="15"/>
+      <c r="AL34" s="15"/>
+      <c r="AM34" s="15"/>
+      <c r="AN34" s="15"/>
+      <c r="AO34" s="15"/>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>22</v>
       </c>
@@ -1700,29 +2981,67 @@
         <f>AVERAGE(O35:S35)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35" s="15"/>
+      <c r="V35" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="8"/>
+      <c r="AC35" s="5" t="e">
+        <f>AVERAGE(X35:AB35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD35" s="6"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="8"/>
+      <c r="AI35" s="5" t="e">
+        <f>AVERAGE(AD35:AH35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="8"/>
+      <c r="AO35" s="5" t="e">
+        <f>AVERAGE(AJ35:AN35)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="9">
+        <v>2467.232</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="5" t="e">
-        <f t="shared" ref="H36:H43" si="9">AVERAGE(C36:G36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36" s="9"/>
+      <c r="H36" s="5">
+        <f t="shared" ref="H36:H43" si="18">AVERAGE(C36:G36)</f>
+        <v>2467.232</v>
+      </c>
+      <c r="I36" s="9">
+        <v>1584.7449999999999</v>
+      </c>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="11"/>
-      <c r="N36" s="5" t="e">
-        <f t="shared" ref="N36:N43" si="10">AVERAGE(I36:M36)</f>
-        <v>#DIV/0!</v>
+      <c r="N36" s="5">
+        <f t="shared" ref="N36:N43" si="19">AVERAGE(I36:M36)</f>
+        <v>1584.7449999999999</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="10"/>
@@ -1730,31 +3049,71 @@
       <c r="R36" s="10"/>
       <c r="S36" s="11"/>
       <c r="T36" s="5" t="e">
-        <f t="shared" ref="T36:T43" si="11">AVERAGE(O36:S36)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T36:T43" si="20">AVERAGE(O36:S36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U36" s="15"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X36" s="9">
+        <v>2.383</v>
+      </c>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="10"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="5">
+        <f t="shared" ref="AC36:AC43" si="21">AVERAGE(X36:AB36)</f>
+        <v>2.383</v>
+      </c>
+      <c r="AD36" s="9">
+        <v>3.7109999999999999</v>
+      </c>
+      <c r="AE36" s="10"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
+      <c r="AH36" s="11"/>
+      <c r="AI36" s="5">
+        <f t="shared" ref="AI36:AI43" si="22">AVERAGE(AD36:AH36)</f>
+        <v>3.7109999999999999</v>
+      </c>
+      <c r="AJ36" s="9"/>
+      <c r="AK36" s="10"/>
+      <c r="AL36" s="10"/>
+      <c r="AM36" s="10"/>
+      <c r="AN36" s="11"/>
+      <c r="AO36" s="5" t="e">
+        <f t="shared" ref="AO36:AO43" si="23">AVERAGE(AJ36:AN36)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="11"/>
       <c r="H37" s="5" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I37" s="9"/>
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="11"/>
       <c r="N37" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O37" s="9"/>
@@ -1763,31 +3122,87 @@
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
       <c r="T37" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U37" s="15"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X37" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC37" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD37" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI37" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ37" s="9"/>
+      <c r="AK37" s="10"/>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="10"/>
+      <c r="AN37" s="11"/>
+      <c r="AO37" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="11"/>
       <c r="H38" s="5" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I38" s="9"/>
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="11"/>
       <c r="N38" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O38" s="9"/>
@@ -1796,31 +3211,87 @@
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
       <c r="T38" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U38" s="15"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X38" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC38" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD38" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI38" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ38" s="9"/>
+      <c r="AK38" s="10"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="10"/>
+      <c r="AN38" s="11"/>
+      <c r="AO38" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="9"/>
+      <c r="C39" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
       <c r="H39" s="5" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I39" s="9"/>
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="11"/>
       <c r="N39" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O39" s="9"/>
@@ -1829,11 +3300,63 @@
       <c r="R39" s="10"/>
       <c r="S39" s="11"/>
       <c r="T39" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U39" s="15"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X39" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC39" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD39" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI39" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ39" s="9"/>
+      <c r="AK39" s="10"/>
+      <c r="AL39" s="10"/>
+      <c r="AM39" s="10"/>
+      <c r="AN39" s="11"/>
+      <c r="AO39" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
@@ -1844,7 +3367,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="11"/>
       <c r="H40" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" s="9"/>
@@ -1853,7 +3376,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="11"/>
       <c r="N40" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O40" s="9"/>
@@ -1862,11 +3385,43 @@
       <c r="R40" s="10"/>
       <c r="S40" s="11"/>
       <c r="T40" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U40" s="15"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="10"/>
+      <c r="AB40" s="11"/>
+      <c r="AC40" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="10"/>
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="10"/>
+      <c r="AH40" s="11"/>
+      <c r="AI40" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ40" s="9"/>
+      <c r="AK40" s="10"/>
+      <c r="AL40" s="10"/>
+      <c r="AM40" s="10"/>
+      <c r="AN40" s="11"/>
+      <c r="AO40" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
       <c r="B41" s="4" t="s">
         <v>7</v>
@@ -1877,7 +3432,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="11"/>
       <c r="H41" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" s="9"/>
@@ -1886,7 +3441,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="11"/>
       <c r="N41" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O41" s="9"/>
@@ -1895,11 +3450,43 @@
       <c r="R41" s="10"/>
       <c r="S41" s="11"/>
       <c r="T41" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U41" s="15"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="10"/>
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="10"/>
+      <c r="AH41" s="11"/>
+      <c r="AI41" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ41" s="9"/>
+      <c r="AK41" s="10"/>
+      <c r="AL41" s="10"/>
+      <c r="AM41" s="10"/>
+      <c r="AN41" s="11"/>
+      <c r="AO41" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" s="4" t="s">
         <v>8</v>
@@ -1910,7 +3497,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="11"/>
       <c r="H42" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" s="9"/>
@@ -1919,7 +3506,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="11"/>
       <c r="N42" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O42" s="9"/>
@@ -1928,11 +3515,43 @@
       <c r="R42" s="10"/>
       <c r="S42" s="11"/>
       <c r="T42" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U42" s="15"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD42" s="9"/>
+      <c r="AE42" s="10"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="10"/>
+      <c r="AH42" s="11"/>
+      <c r="AI42" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ42" s="9"/>
+      <c r="AK42" s="10"/>
+      <c r="AL42" s="10"/>
+      <c r="AM42" s="10"/>
+      <c r="AN42" s="11"/>
+      <c r="AO42" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="4" t="s">
         <v>9</v>
@@ -1943,7 +3562,7 @@
       <c r="F43" s="13"/>
       <c r="G43" s="14"/>
       <c r="H43" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" s="12"/>
@@ -1952,7 +3571,7 @@
       <c r="L43" s="13"/>
       <c r="M43" s="14"/>
       <c r="N43" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O43" s="12"/>
@@ -1961,27 +3580,59 @@
       <c r="R43" s="13"/>
       <c r="S43" s="14"/>
       <c r="T43" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U43" s="15"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X43" s="12"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD43" s="12"/>
+      <c r="AE43" s="13"/>
+      <c r="AF43" s="13"/>
+      <c r="AG43" s="13"/>
+      <c r="AH43" s="14"/>
+      <c r="AI43" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ43" s="12"/>
+      <c r="AK43" s="13"/>
+      <c r="AL43" s="13"/>
+      <c r="AM43" s="13"/>
+      <c r="AN43" s="14"/>
+      <c r="AO43" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
     </row>
@@ -2126,15 +3777,23 @@
       <c r="B83"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
+    <mergeCell ref="V15:V23"/>
+    <mergeCell ref="V25:V33"/>
+    <mergeCell ref="V35:V43"/>
+    <mergeCell ref="V1:X2"/>
+    <mergeCell ref="X3:AC3"/>
+    <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="AJ3:AO3"/>
+    <mergeCell ref="V5:V13"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="A35:A43"/>
     <mergeCell ref="O3:T3"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:N3"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="A35:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunti valori bf1 più veloci bf1 su GTX1070
</commit_message>
<xml_diff>
--- a/performance bf1.xlsx
+++ b/performance bf1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D780041-7A07-463B-A113-BF7FEED43CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF26AFB-4F23-46E8-9C62-105BB6229FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="270" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,12 +319,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -607,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD37" sqref="AD37:AH39"/>
+    <sheetView tabSelected="1" topLeftCell="AA25" workbookViewId="0">
+      <selection activeCell="AI43" sqref="AI43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,78 +620,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="V1" s="21" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="V1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
     </row>
     <row r="3" spans="1:41" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="15"/>
       <c r="V3" s="17"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="20" t="s">
+      <c r="X3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20" t="s">
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20" t="s">
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="20"/>
-      <c r="AO3" s="20"/>
+      <c r="AK3" s="21"/>
+      <c r="AL3" s="21"/>
+      <c r="AM3" s="21"/>
+      <c r="AN3" s="21"/>
+      <c r="AO3" s="21"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -821,14 +822,24 @@
         <f>AVERAGE(C5:G5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="5" t="e">
+      <c r="I5" s="6">
+        <v>9.5519999999999996</v>
+      </c>
+      <c r="J5" s="7">
+        <v>9.4570000000000007</v>
+      </c>
+      <c r="K5" s="7">
+        <v>9.4640000000000004</v>
+      </c>
+      <c r="L5" s="7">
+        <v>9.4610000000000003</v>
+      </c>
+      <c r="M5" s="8">
+        <v>9.5310000000000006</v>
+      </c>
+      <c r="N5" s="5">
         <f>AVERAGE(I5:M5)</f>
-        <v>#DIV/0!</v>
+        <v>9.4929999999999986</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="7"/>
@@ -855,14 +866,24 @@
         <f>AVERAGE(X5:AB5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="5" t="e">
+      <c r="AD5" s="6">
+        <v>3.11</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>3.141</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>3.1389999999999998</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>3.14</v>
+      </c>
+      <c r="AH5" s="8">
+        <v>3.1160000000000001</v>
+      </c>
+      <c r="AI5" s="5">
         <f>AVERAGE(AD5:AH5)</f>
-        <v>#DIV/0!</v>
+        <v>3.1292</v>
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="7"/>
@@ -1236,14 +1257,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="5" t="e">
+      <c r="I10" s="9">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="J10" s="10">
+        <v>1.4059999999999999</v>
+      </c>
+      <c r="K10" s="10">
+        <v>1.377</v>
+      </c>
+      <c r="L10" s="22">
+        <v>1.403</v>
+      </c>
+      <c r="M10" s="11">
+        <v>1.4039999999999999</v>
+      </c>
+      <c r="N10" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.411</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="10"/>
@@ -1268,14 +1299,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="5" t="e">
+      <c r="AD10" s="9">
+        <v>170.5</v>
+      </c>
+      <c r="AE10" s="10">
+        <v>177.7</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>181.4</v>
+      </c>
+      <c r="AG10" s="22">
+        <v>178</v>
+      </c>
+      <c r="AH10" s="11">
+        <v>178</v>
+      </c>
+      <c r="AI10" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>177.12</v>
       </c>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="10"/>
@@ -1301,14 +1342,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="5" t="e">
+      <c r="I11" s="9">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1.556</v>
+      </c>
+      <c r="K11" s="10">
+        <v>1.5409999999999999</v>
+      </c>
+      <c r="L11" s="22">
+        <v>1.538</v>
+      </c>
+      <c r="M11" s="11">
+        <v>1.55</v>
+      </c>
+      <c r="N11" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.5562</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="10"/>
@@ -1333,14 +1384,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="10"/>
-      <c r="AF11" s="10"/>
-      <c r="AG11" s="10"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="5" t="e">
+      <c r="AD11" s="9">
+        <v>313.10000000000002</v>
+      </c>
+      <c r="AE11" s="10">
+        <v>321</v>
+      </c>
+      <c r="AF11" s="10">
+        <v>324.10000000000002</v>
+      </c>
+      <c r="AG11" s="22">
+        <v>324.8</v>
+      </c>
+      <c r="AH11" s="11">
+        <v>322.39999999999998</v>
+      </c>
+      <c r="AI11" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>321.08000000000004</v>
       </c>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="10"/>
@@ -1366,14 +1427,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="5" t="e">
+      <c r="I12" s="9">
+        <v>1.5880000000000001</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1.544</v>
+      </c>
+      <c r="K12" s="10">
+        <v>1.5289999999999999</v>
+      </c>
+      <c r="L12" s="22">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="M12" s="11">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="N12" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.5509999999999997</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="10"/>
@@ -1398,14 +1469,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="10"/>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="5" t="e">
+      <c r="AD12" s="9">
+        <v>471.9</v>
+      </c>
+      <c r="AE12" s="10">
+        <v>485.1</v>
+      </c>
+      <c r="AF12" s="10">
+        <v>490.1</v>
+      </c>
+      <c r="AG12" s="22">
+        <v>481.9</v>
+      </c>
+      <c r="AH12" s="11">
+        <v>486.7</v>
+      </c>
+      <c r="AI12" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>483.14</v>
       </c>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="10"/>
@@ -1431,14 +1512,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="5" t="e">
+      <c r="I13" s="12">
+        <v>1.6140000000000001</v>
+      </c>
+      <c r="J13" s="13">
+        <v>1.569</v>
+      </c>
+      <c r="K13" s="13">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="L13" s="13">
+        <v>1.577</v>
+      </c>
+      <c r="M13" s="14">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="N13" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.5783999999999998</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="13"/>
@@ -1463,14 +1554,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="5" t="e">
+      <c r="AD13" s="12">
+        <v>619</v>
+      </c>
+      <c r="AE13" s="13">
+        <v>636.5</v>
+      </c>
+      <c r="AF13" s="13">
+        <v>638.1</v>
+      </c>
+      <c r="AG13" s="13">
+        <v>633.6</v>
+      </c>
+      <c r="AH13" s="14">
+        <v>638.1</v>
+      </c>
+      <c r="AI13" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>633.05999999999995</v>
       </c>
       <c r="AJ13" s="12"/>
       <c r="AK13" s="13"/>
@@ -1541,14 +1642,24 @@
         <f>AVERAGE(C15:G15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="5" t="e">
+      <c r="I15" s="6">
+        <v>7.7939999999999996</v>
+      </c>
+      <c r="J15" s="7">
+        <v>7.74</v>
+      </c>
+      <c r="K15" s="7">
+        <v>7.726</v>
+      </c>
+      <c r="L15" s="7">
+        <v>7.7409999999999997</v>
+      </c>
+      <c r="M15" s="8">
+        <v>7.7350000000000003</v>
+      </c>
+      <c r="N15" s="5">
         <f>AVERAGE(I15:M15)</f>
-        <v>#DIV/0!</v>
+        <v>7.7471999999999994</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="7"/>
@@ -1575,14 +1686,24 @@
         <f>AVERAGE(X15:AB15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="5" t="e">
+      <c r="AD15" s="6">
+        <v>3.8109999999999999</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>3.8380000000000001</v>
+      </c>
+      <c r="AF15" s="7">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="AG15" s="7">
+        <v>3.8370000000000002</v>
+      </c>
+      <c r="AH15" s="8">
+        <v>3.84</v>
+      </c>
+      <c r="AI15" s="5">
         <f>AVERAGE(AD15:AH15)</f>
-        <v>#DIV/0!</v>
+        <v>3.8342000000000001</v>
       </c>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="7"/>
@@ -1937,23 +2058,28 @@
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
       <c r="H20" s="5" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="5" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <f>AVERAGE(C20:G20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1.288</v>
+      </c>
+      <c r="J20" s="10">
+        <v>1.254</v>
+      </c>
+      <c r="K20" s="10">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="L20" s="22">
+        <v>1.234</v>
+      </c>
+      <c r="M20" s="11">
+        <v>1.25</v>
+      </c>
+      <c r="N20" s="5">
+        <f>AVERAGE(I20:M20)</f>
+        <v>1.2538</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="10"/>
@@ -1978,14 +2104,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
-      <c r="AH20" s="11"/>
-      <c r="AI20" s="5" t="e">
+      <c r="AD20" s="9">
+        <v>193.9</v>
+      </c>
+      <c r="AE20" s="10">
+        <v>199.2</v>
+      </c>
+      <c r="AF20" s="10">
+        <v>201</v>
+      </c>
+      <c r="AG20" s="22">
+        <v>202.4</v>
+      </c>
+      <c r="AH20" s="11">
+        <v>199.9</v>
+      </c>
+      <c r="AI20" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>199.28</v>
       </c>
       <c r="AJ20" s="9"/>
       <c r="AK20" s="10"/>
@@ -2011,14 +2147,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="5" t="e">
+      <c r="I21" s="9">
+        <v>1.42</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1.359</v>
+      </c>
+      <c r="K21" s="10">
+        <v>1.319</v>
+      </c>
+      <c r="L21" s="22">
+        <v>1.35</v>
+      </c>
+      <c r="M21" s="11">
+        <v>1.36</v>
+      </c>
+      <c r="N21" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1.3616000000000001</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="10"/>
@@ -2043,14 +2189,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="10"/>
-      <c r="AG21" s="10"/>
-      <c r="AH21" s="11"/>
-      <c r="AI21" s="5" t="e">
+      <c r="AD21" s="9">
+        <v>351.8</v>
+      </c>
+      <c r="AE21" s="10">
+        <v>367.5</v>
+      </c>
+      <c r="AF21" s="10">
+        <v>378.7</v>
+      </c>
+      <c r="AG21" s="22">
+        <v>370.1</v>
+      </c>
+      <c r="AH21" s="11">
+        <v>367.2</v>
+      </c>
+      <c r="AI21" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>367.06</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="10"/>
@@ -2076,14 +2232,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="5" t="e">
+      <c r="I22" s="9">
+        <v>1.444</v>
+      </c>
+      <c r="J22" s="10">
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="K22" s="10">
+        <v>1.38</v>
+      </c>
+      <c r="L22" s="22">
+        <v>1.395</v>
+      </c>
+      <c r="M22" s="11">
+        <v>1.3919999999999999</v>
+      </c>
+      <c r="N22" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1.3997999999999997</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="10"/>
@@ -2108,14 +2274,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="10"/>
-      <c r="AF22" s="10"/>
-      <c r="AG22" s="10"/>
-      <c r="AH22" s="11"/>
-      <c r="AI22" s="5" t="e">
+      <c r="AD22" s="9">
+        <v>519</v>
+      </c>
+      <c r="AE22" s="10">
+        <v>540</v>
+      </c>
+      <c r="AF22" s="10">
+        <v>542.79999999999995</v>
+      </c>
+      <c r="AG22" s="22">
+        <v>537.20000000000005</v>
+      </c>
+      <c r="AH22" s="11">
+        <v>538.1</v>
+      </c>
+      <c r="AI22" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>535.41999999999996</v>
       </c>
       <c r="AJ22" s="9"/>
       <c r="AK22" s="10"/>
@@ -2141,14 +2317,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="5" t="e">
+      <c r="I23" s="12">
+        <v>1.472</v>
+      </c>
+      <c r="J23" s="13">
+        <v>1.429</v>
+      </c>
+      <c r="K23" s="13">
+        <v>1.43</v>
+      </c>
+      <c r="L23" s="13">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="M23" s="14">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="N23" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1.4375999999999998</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="13"/>
@@ -2173,14 +2359,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD23" s="12"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="14"/>
-      <c r="AI23" s="5" t="e">
+      <c r="AD23" s="12">
+        <v>678.5</v>
+      </c>
+      <c r="AE23" s="13">
+        <v>698.9</v>
+      </c>
+      <c r="AF23" s="13">
+        <v>698.5</v>
+      </c>
+      <c r="AG23" s="13">
+        <v>702.4</v>
+      </c>
+      <c r="AH23" s="14">
+        <v>696</v>
+      </c>
+      <c r="AI23" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>694.86</v>
       </c>
       <c r="AJ23" s="12"/>
       <c r="AK23" s="13"/>
@@ -2251,14 +2447,24 @@
         <f>AVERAGE(C25:G25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="5" t="e">
+      <c r="I25" s="6">
+        <v>8.2040000000000006</v>
+      </c>
+      <c r="J25" s="7">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="K25" s="7">
+        <v>8.1150000000000002</v>
+      </c>
+      <c r="L25" s="7">
+        <v>8.1140000000000008</v>
+      </c>
+      <c r="M25" s="8">
+        <v>8.1050000000000004</v>
+      </c>
+      <c r="N25" s="5">
         <f>AVERAGE(I25:M25)</f>
-        <v>#DIV/0!</v>
+        <v>8.1336000000000013</v>
       </c>
       <c r="O25" s="6"/>
       <c r="P25" s="7"/>
@@ -2285,14 +2491,24 @@
         <f>AVERAGE(X25:AB25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="7"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="7"/>
-      <c r="AH25" s="8"/>
-      <c r="AI25" s="5" t="e">
+      <c r="AD25" s="6">
+        <v>3.621</v>
+      </c>
+      <c r="AE25" s="7">
+        <v>3.6539999999999999</v>
+      </c>
+      <c r="AF25" s="7">
+        <v>3.661</v>
+      </c>
+      <c r="AG25" s="7">
+        <v>3.661</v>
+      </c>
+      <c r="AH25" s="8">
+        <v>3.665</v>
+      </c>
+      <c r="AI25" s="5">
         <f>AVERAGE(AD25:AH25)</f>
-        <v>#DIV/0!</v>
+        <v>3.6524000000000001</v>
       </c>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="7"/>
@@ -2658,14 +2874,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="5" t="e">
+      <c r="I30" s="9">
+        <v>1.069</v>
+      </c>
+      <c r="J30" s="10">
+        <v>1.01</v>
+      </c>
+      <c r="K30" s="10">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="L30" s="22">
+        <v>1</v>
+      </c>
+      <c r="M30" s="11">
+        <v>1</v>
+      </c>
+      <c r="N30" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>1.0187999999999999</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="10"/>
@@ -2690,14 +2916,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="10"/>
-      <c r="AF30" s="10"/>
-      <c r="AG30" s="10"/>
-      <c r="AH30" s="11"/>
-      <c r="AI30" s="5" t="e">
+      <c r="AD30" s="9">
+        <v>233.7</v>
+      </c>
+      <c r="AE30" s="10">
+        <v>247.4</v>
+      </c>
+      <c r="AF30" s="10">
+        <v>246.1</v>
+      </c>
+      <c r="AG30" s="22">
+        <v>249.8</v>
+      </c>
+      <c r="AH30" s="11">
+        <v>249.9</v>
+      </c>
+      <c r="AI30" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>245.38000000000002</v>
       </c>
       <c r="AJ30" s="9"/>
       <c r="AK30" s="10"/>
@@ -2723,14 +2959,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="5" t="e">
+      <c r="I31" s="9">
+        <v>1.3640000000000001</v>
+      </c>
+      <c r="J31" s="10">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="K31" s="10">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="L31" s="22">
+        <v>1.06</v>
+      </c>
+      <c r="M31" s="11">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="N31" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>1.2664000000000002</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="10"/>
@@ -2755,14 +3001,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="10"/>
-      <c r="AF31" s="10"/>
-      <c r="AG31" s="10"/>
-      <c r="AH31" s="11"/>
-      <c r="AI31" s="5" t="e">
+      <c r="AD31" s="9">
+        <v>366.2</v>
+      </c>
+      <c r="AE31" s="10">
+        <v>388.9</v>
+      </c>
+      <c r="AF31" s="10">
+        <v>381.7</v>
+      </c>
+      <c r="AG31" s="22">
+        <v>382.6</v>
+      </c>
+      <c r="AH31" s="11">
+        <v>380.3</v>
+      </c>
+      <c r="AI31" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>379.94</v>
       </c>
       <c r="AJ31" s="9"/>
       <c r="AK31" s="10"/>
@@ -2788,14 +3044,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="5" t="e">
+      <c r="I32" s="9">
+        <v>1.401</v>
+      </c>
+      <c r="J32" s="10">
+        <v>1.3380000000000001</v>
+      </c>
+      <c r="K32" s="10">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="L32" s="22">
+        <v>1.3169999999999999</v>
+      </c>
+      <c r="M32" s="11">
+        <v>1.329</v>
+      </c>
+      <c r="N32" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>1.3426</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="10"/>
@@ -2820,14 +3086,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="10"/>
-      <c r="AF32" s="10"/>
-      <c r="AG32" s="10"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="5" t="e">
+      <c r="AD32" s="9">
+        <v>535</v>
+      </c>
+      <c r="AE32" s="10">
+        <v>560.1</v>
+      </c>
+      <c r="AF32" s="10">
+        <v>564.4</v>
+      </c>
+      <c r="AG32" s="22">
+        <v>569</v>
+      </c>
+      <c r="AH32" s="11">
+        <v>563.70000000000005</v>
+      </c>
+      <c r="AI32" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>558.43999999999994</v>
       </c>
       <c r="AJ32" s="9"/>
       <c r="AK32" s="10"/>
@@ -2853,14 +3129,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="5" t="e">
+      <c r="I33" s="12">
+        <v>1.413</v>
+      </c>
+      <c r="J33" s="13">
+        <v>1.3580000000000001</v>
+      </c>
+      <c r="K33" s="13">
+        <v>1.361</v>
+      </c>
+      <c r="L33" s="13">
+        <v>1.353</v>
+      </c>
+      <c r="M33" s="14">
+        <v>1.359</v>
+      </c>
+      <c r="N33" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>1.3687999999999998</v>
       </c>
       <c r="O33" s="12"/>
       <c r="P33" s="13"/>
@@ -2885,14 +3171,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD33" s="12"/>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
-      <c r="AH33" s="14"/>
-      <c r="AI33" s="5" t="e">
+      <c r="AD33" s="12">
+        <v>707.2</v>
+      </c>
+      <c r="AE33" s="13">
+        <v>735.7</v>
+      </c>
+      <c r="AF33" s="13">
+        <v>734.3</v>
+      </c>
+      <c r="AG33" s="13">
+        <v>738.6</v>
+      </c>
+      <c r="AH33" s="14">
+        <v>735.2</v>
+      </c>
+      <c r="AI33" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>730.2</v>
       </c>
       <c r="AJ33" s="12"/>
       <c r="AK33" s="13"/>
@@ -2963,14 +3259,24 @@
         <f>AVERAGE(C35:G35)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="5" t="e">
+      <c r="I35" s="6">
+        <v>7.6390000000000002</v>
+      </c>
+      <c r="J35" s="7">
+        <v>7.5629999999999997</v>
+      </c>
+      <c r="K35" s="7">
+        <v>7.5650000000000004</v>
+      </c>
+      <c r="L35" s="7">
+        <v>7.57</v>
+      </c>
+      <c r="M35" s="8">
+        <v>7.5449999999999999</v>
+      </c>
+      <c r="N35" s="5">
         <f>AVERAGE(I35:M35)</f>
-        <v>#DIV/0!</v>
+        <v>7.5763999999999996</v>
       </c>
       <c r="O35" s="6"/>
       <c r="P35" s="7"/>
@@ -2997,14 +3303,24 @@
         <f>AVERAGE(X35:AB35)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD35" s="6"/>
-      <c r="AE35" s="7"/>
-      <c r="AF35" s="7"/>
-      <c r="AG35" s="7"/>
-      <c r="AH35" s="8"/>
-      <c r="AI35" s="5" t="e">
+      <c r="AD35" s="6">
+        <v>3.8889999999999998</v>
+      </c>
+      <c r="AE35" s="7">
+        <v>3.9279999999999999</v>
+      </c>
+      <c r="AF35" s="7">
+        <v>3.9260000000000002</v>
+      </c>
+      <c r="AG35" s="7">
+        <v>3.9239999999999999</v>
+      </c>
+      <c r="AH35" s="8">
+        <v>3.9369999999999998</v>
+      </c>
+      <c r="AI35" s="5">
         <f>AVERAGE(AD35:AH35)</f>
-        <v>#DIV/0!</v>
+        <v>3.9207999999999998</v>
       </c>
       <c r="AJ35" s="6"/>
       <c r="AK35" s="7"/>
@@ -3370,14 +3686,24 @@
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="9"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="5" t="e">
+      <c r="I40" s="9">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="J40" s="10">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K40" s="10">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="L40" s="22">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="M40" s="11">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="N40" s="5">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
+        <v>0.95599999999999985</v>
       </c>
       <c r="O40" s="9"/>
       <c r="P40" s="10"/>
@@ -3402,14 +3728,24 @@
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD40" s="9"/>
-      <c r="AE40" s="10"/>
-      <c r="AF40" s="10"/>
-      <c r="AG40" s="10"/>
-      <c r="AH40" s="11"/>
-      <c r="AI40" s="5" t="e">
+      <c r="AD40" s="9">
+        <v>242.8</v>
+      </c>
+      <c r="AE40" s="10">
+        <v>270.3</v>
+      </c>
+      <c r="AF40" s="10">
+        <v>266.39999999999998</v>
+      </c>
+      <c r="AG40" s="22">
+        <v>266.3</v>
+      </c>
+      <c r="AH40" s="11">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="AI40" s="5">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>261.68</v>
       </c>
       <c r="AJ40" s="9"/>
       <c r="AK40" s="10"/>
@@ -3435,14 +3771,24 @@
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="9"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="5" t="e">
+      <c r="I41" s="9">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="J41" s="10">
+        <v>1.2210000000000001</v>
+      </c>
+      <c r="K41" s="10">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="L41" s="22">
+        <v>1.232</v>
+      </c>
+      <c r="M41" s="11">
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="N41" s="5">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
+        <v>1.2432000000000001</v>
       </c>
       <c r="O41" s="9"/>
       <c r="P41" s="10"/>
@@ -3467,14 +3813,24 @@
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD41" s="9"/>
-      <c r="AE41" s="10"/>
-      <c r="AF41" s="10"/>
-      <c r="AG41" s="10"/>
-      <c r="AH41" s="11"/>
-      <c r="AI41" s="5" t="e">
+      <c r="AD41" s="9">
+        <v>385</v>
+      </c>
+      <c r="AE41" s="10">
+        <v>409.2</v>
+      </c>
+      <c r="AF41" s="10">
+        <v>405.7</v>
+      </c>
+      <c r="AG41" s="22">
+        <v>405.6</v>
+      </c>
+      <c r="AH41" s="11">
+        <v>404.6</v>
+      </c>
+      <c r="AI41" s="5">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>402.02</v>
       </c>
       <c r="AJ41" s="9"/>
       <c r="AK41" s="10"/>
@@ -3500,14 +3856,24 @@
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="9"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="5" t="e">
+      <c r="I42" s="9">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="J42" s="10">
+        <v>1.254</v>
+      </c>
+      <c r="K42" s="10">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="L42" s="22">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="M42" s="11">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="N42" s="5">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
+        <v>1.2724</v>
       </c>
       <c r="O42" s="9"/>
       <c r="P42" s="10"/>
@@ -3532,14 +3898,24 @@
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD42" s="9"/>
-      <c r="AE42" s="10"/>
-      <c r="AF42" s="10"/>
-      <c r="AG42" s="10"/>
-      <c r="AH42" s="11"/>
-      <c r="AI42" s="5" t="e">
+      <c r="AD42" s="9">
+        <v>577.79999999999995</v>
+      </c>
+      <c r="AE42" s="10">
+        <v>597.5</v>
+      </c>
+      <c r="AF42" s="10">
+        <v>591.6</v>
+      </c>
+      <c r="AG42" s="22">
+        <v>591.29999999999995</v>
+      </c>
+      <c r="AH42" s="11">
+        <v>586.6</v>
+      </c>
+      <c r="AI42" s="5">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>588.95999999999992</v>
       </c>
       <c r="AJ42" s="9"/>
       <c r="AK42" s="10"/>
@@ -3565,14 +3941,24 @@
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="5" t="e">
+      <c r="I43" s="12">
+        <v>1.36</v>
+      </c>
+      <c r="J43" s="13">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="K43" s="13">
+        <v>1.302</v>
+      </c>
+      <c r="L43" s="13">
+        <v>1.31</v>
+      </c>
+      <c r="M43" s="14">
+        <v>1.284</v>
+      </c>
+      <c r="N43" s="5">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
+        <v>1.3122</v>
       </c>
       <c r="O43" s="12"/>
       <c r="P43" s="13"/>
@@ -3597,14 +3983,24 @@
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD43" s="12"/>
-      <c r="AE43" s="13"/>
-      <c r="AF43" s="13"/>
-      <c r="AG43" s="13"/>
-      <c r="AH43" s="14"/>
-      <c r="AI43" s="5" t="e">
+      <c r="AD43" s="12">
+        <v>734.5</v>
+      </c>
+      <c r="AE43" s="13">
+        <v>765.3</v>
+      </c>
+      <c r="AF43" s="13">
+        <v>767.4</v>
+      </c>
+      <c r="AG43" s="13">
+        <v>762.8</v>
+      </c>
+      <c r="AH43" s="14">
+        <v>777.8</v>
+      </c>
+      <c r="AI43" s="5">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>761.56000000000006</v>
       </c>
       <c r="AJ43" s="12"/>
       <c r="AK43" s="13"/>
@@ -3778,11 +4174,10 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="V15:V23"/>
-    <mergeCell ref="V25:V33"/>
-    <mergeCell ref="V35:V43"/>
-    <mergeCell ref="V1:X2"/>
-    <mergeCell ref="X3:AC3"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:N3"/>
     <mergeCell ref="AD3:AI3"/>
     <mergeCell ref="AJ3:AO3"/>
     <mergeCell ref="V5:V13"/>
@@ -3790,10 +4185,11 @@
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="O3:T3"/>
     <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="V15:V23"/>
+    <mergeCell ref="V25:V33"/>
+    <mergeCell ref="V35:V43"/>
+    <mergeCell ref="V1:X2"/>
+    <mergeCell ref="X3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunti valori bf1 per 940MX
</commit_message>
<xml_diff>
--- a/performance bf1.xlsx
+++ b/performance bf1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF26AFB-4F23-46E8-9C62-105BB6229FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308C29CB-9A73-4DA5-B634-A2C2D826FDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="270" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="26">
   <si>
     <t>SPEEDUP</t>
   </si>
@@ -316,16 +316,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA25" workbookViewId="0">
-      <selection activeCell="AI43" sqref="AI43"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,78 +620,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="V1" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="V1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
     </row>
     <row r="3" spans="1:41" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
       <c r="U3" s="15"/>
       <c r="V3" s="17"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="21" t="s">
+      <c r="X3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21" t="s">
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21" t="s">
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -807,20 +807,30 @@
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="5" t="e">
+      <c r="C5" s="6">
+        <v>13.538</v>
+      </c>
+      <c r="D5" s="7">
+        <v>13.348000000000001</v>
+      </c>
+      <c r="E5" s="7">
+        <v>13.525</v>
+      </c>
+      <c r="F5" s="7">
+        <v>13.317</v>
+      </c>
+      <c r="G5" s="8">
+        <v>13.420999999999999</v>
+      </c>
+      <c r="H5" s="5">
         <f>AVERAGE(C5:G5)</f>
-        <v>#DIV/0!</v>
+        <v>13.4298</v>
       </c>
       <c r="I5" s="6">
         <v>9.5519999999999996</v>
@@ -851,20 +861,30 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U5" s="15"/>
-      <c r="V5" s="19" t="s">
+      <c r="V5" s="21" t="s">
         <v>19</v>
       </c>
       <c r="W5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="5" t="e">
+      <c r="X5" s="6">
+        <v>2.194</v>
+      </c>
+      <c r="Y5" s="7">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>2.1960000000000002</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>2.2309999999999999</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>2.2130000000000001</v>
+      </c>
+      <c r="AC5" s="5">
         <f>AVERAGE(X5:AB5)</f>
-        <v>#DIV/0!</v>
+        <v>2.2118000000000002</v>
       </c>
       <c r="AD5" s="6">
         <v>3.11</v>
@@ -896,17 +916,25 @@
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="5" t="e">
         <f t="shared" ref="H6:H13" si="0">AVERAGE(C6:G6)</f>
         <v>#DIV/0!</v>
@@ -932,7 +960,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U6" s="15"/>
-      <c r="V6" s="19"/>
+      <c r="V6" s="21"/>
       <c r="W6" s="4" t="s">
         <v>2</v>
       </c>
@@ -977,17 +1005,25 @@
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -995,10 +1031,18 @@
       <c r="I7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11"/>
+      <c r="J7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N7" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -1013,7 +1057,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U7" s="15"/>
-      <c r="V7" s="19"/>
+      <c r="V7" s="21"/>
       <c r="W7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1066,17 +1110,25 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1084,10 +1136,18 @@
       <c r="I8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="11"/>
+      <c r="J8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N8" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -1102,7 +1162,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U8" s="15"/>
-      <c r="V8" s="19"/>
+      <c r="V8" s="21"/>
       <c r="W8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1155,17 +1215,25 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H9" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1173,10 +1241,18 @@
       <c r="I9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="11"/>
+      <c r="J9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N9" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -1191,7 +1267,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U9" s="15"/>
-      <c r="V9" s="19"/>
+      <c r="V9" s="21"/>
       <c r="W9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1244,18 +1320,28 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="5" t="e">
+      <c r="C10" s="9">
+        <v>2.1739999999999999</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2.2290000000000001</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.903</v>
+      </c>
+      <c r="F10" s="19">
+        <v>2.008</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1.905</v>
+      </c>
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.0438000000000001</v>
       </c>
       <c r="I10" s="9">
         <v>1.4650000000000001</v>
@@ -1266,7 +1352,7 @@
       <c r="K10" s="10">
         <v>1.377</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="19">
         <v>1.403</v>
       </c>
       <c r="M10" s="11">
@@ -1286,18 +1372,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U10" s="15"/>
-      <c r="V10" s="19"/>
+      <c r="V10" s="21"/>
       <c r="W10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="5" t="e">
+      <c r="X10" s="9">
+        <v>114.9</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>112.1</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>131.30000000000001</v>
+      </c>
+      <c r="AA10" s="19">
+        <v>124.4</v>
+      </c>
+      <c r="AB10" s="11">
+        <v>131.1</v>
+      </c>
+      <c r="AC10" s="5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>122.76000000000002</v>
       </c>
       <c r="AD10" s="9">
         <v>170.5</v>
@@ -1308,7 +1404,7 @@
       <c r="AF10" s="10">
         <v>181.4</v>
       </c>
-      <c r="AG10" s="22">
+      <c r="AG10" s="19">
         <v>178</v>
       </c>
       <c r="AH10" s="11">
@@ -1329,18 +1425,28 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="5" t="e">
+      <c r="C11" s="9">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D11" s="10">
+        <v>2.028</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2.0169999999999999</v>
+      </c>
+      <c r="F11" s="19">
+        <v>2.048</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.0289999999999999</v>
       </c>
       <c r="I11" s="9">
         <v>1.5960000000000001</v>
@@ -1351,7 +1457,7 @@
       <c r="K11" s="10">
         <v>1.5409999999999999</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="19">
         <v>1.538</v>
       </c>
       <c r="M11" s="11">
@@ -1371,18 +1477,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U11" s="15"/>
-      <c r="V11" s="19"/>
+      <c r="V11" s="21"/>
       <c r="W11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="5" t="e">
+      <c r="X11" s="9">
+        <v>246.6</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>246.3</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>247.7</v>
+      </c>
+      <c r="AA11" s="19">
+        <v>243.9</v>
+      </c>
+      <c r="AB11" s="11">
+        <v>246.6</v>
+      </c>
+      <c r="AC11" s="5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>246.21999999999997</v>
       </c>
       <c r="AD11" s="9">
         <v>313.10000000000002</v>
@@ -1393,7 +1509,7 @@
       <c r="AF11" s="10">
         <v>324.10000000000002</v>
       </c>
-      <c r="AG11" s="22">
+      <c r="AG11" s="19">
         <v>324.8</v>
       </c>
       <c r="AH11" s="11">
@@ -1414,18 +1530,28 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="5" t="e">
+      <c r="C12" s="9">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2.036</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2.0760000000000001</v>
+      </c>
+      <c r="F12" s="19">
+        <v>2.044</v>
+      </c>
+      <c r="G12" s="11">
+        <v>2.0209999999999999</v>
+      </c>
+      <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.0444000000000004</v>
       </c>
       <c r="I12" s="9">
         <v>1.5880000000000001</v>
@@ -1436,7 +1562,7 @@
       <c r="K12" s="10">
         <v>1.5289999999999999</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="19">
         <v>1.5549999999999999</v>
       </c>
       <c r="M12" s="11">
@@ -1456,18 +1582,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U12" s="15"/>
-      <c r="V12" s="19"/>
+      <c r="V12" s="21"/>
       <c r="W12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="5" t="e">
+      <c r="X12" s="9">
+        <v>366.4</v>
+      </c>
+      <c r="Y12" s="10">
+        <v>368</v>
+      </c>
+      <c r="Z12" s="10">
+        <v>360.9</v>
+      </c>
+      <c r="AA12" s="19">
+        <v>366.6</v>
+      </c>
+      <c r="AB12" s="11">
+        <v>370.7</v>
+      </c>
+      <c r="AC12" s="5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>366.52000000000004</v>
       </c>
       <c r="AD12" s="9">
         <v>471.9</v>
@@ -1478,7 +1614,7 @@
       <c r="AF12" s="10">
         <v>490.1</v>
       </c>
-      <c r="AG12" s="22">
+      <c r="AG12" s="19">
         <v>481.9</v>
       </c>
       <c r="AH12" s="11">
@@ -1499,18 +1635,28 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="5" t="e">
+      <c r="C13" s="12">
+        <v>2.161</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2.1379999999999999</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2.3610000000000002</v>
+      </c>
+      <c r="F13" s="13">
+        <v>2.1269999999999998</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2.3690000000000002</v>
+      </c>
+      <c r="H13" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.2311999999999999</v>
       </c>
       <c r="I13" s="12">
         <v>1.6140000000000001</v>
@@ -1541,18 +1687,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U13" s="15"/>
-      <c r="V13" s="19"/>
+      <c r="V13" s="21"/>
       <c r="W13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="5" t="e">
+      <c r="X13" s="12">
+        <v>462.3</v>
+      </c>
+      <c r="Y13" s="13">
+        <v>467.3</v>
+      </c>
+      <c r="Z13" s="13">
+        <v>423.1</v>
+      </c>
+      <c r="AA13" s="13">
+        <v>469.7</v>
+      </c>
+      <c r="AB13" s="14">
+        <v>421.7</v>
+      </c>
+      <c r="AC13" s="5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>448.82</v>
       </c>
       <c r="AD13" s="12">
         <v>619</v>
@@ -1627,20 +1783,30 @@
       <c r="AO14" s="15"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="5" t="e">
+      <c r="C15" s="6">
+        <v>11.276999999999999</v>
+      </c>
+      <c r="D15" s="7">
+        <v>11.369</v>
+      </c>
+      <c r="E15" s="7">
+        <v>11.259</v>
+      </c>
+      <c r="F15" s="7">
+        <v>11.378</v>
+      </c>
+      <c r="G15" s="8">
+        <v>11.348000000000001</v>
+      </c>
+      <c r="H15" s="5">
         <f>AVERAGE(C15:G15)</f>
-        <v>#DIV/0!</v>
+        <v>11.3262</v>
       </c>
       <c r="I15" s="6">
         <v>7.7939999999999996</v>
@@ -1671,20 +1837,30 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U15" s="15"/>
-      <c r="V15" s="19" t="s">
+      <c r="V15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="W15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="5" t="e">
+      <c r="X15" s="6">
+        <v>2.6339999999999999</v>
+      </c>
+      <c r="Y15" s="7">
+        <v>2.613</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>2.6379999999999999</v>
+      </c>
+      <c r="AA15" s="7">
+        <v>2.6110000000000002</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>2.6179999999999999</v>
+      </c>
+      <c r="AC15" s="5">
         <f>AVERAGE(X15:AB15)</f>
-        <v>#DIV/0!</v>
+        <v>2.6228000000000002</v>
       </c>
       <c r="AD15" s="6">
         <v>3.8109999999999999</v>
@@ -1716,20 +1892,28 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="9">
         <v>3204.047</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
+      <c r="D16" s="19">
+        <v>3204.92</v>
+      </c>
+      <c r="E16" s="19">
+        <v>3204.866</v>
+      </c>
+      <c r="F16" s="19">
+        <v>3204.933</v>
+      </c>
+      <c r="G16" s="11">
+        <v>3205.4789999999998</v>
+      </c>
       <c r="H16" s="5">
         <f t="shared" ref="H16:H23" si="6">AVERAGE(C16:G16)</f>
-        <v>3204.047</v>
+        <v>3204.8489999999997</v>
       </c>
       <c r="I16" s="9">
         <v>2186.4749999999999</v>
@@ -1752,18 +1936,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U16" s="15"/>
-      <c r="V16" s="19"/>
+      <c r="V16" s="21"/>
       <c r="W16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="5" t="e">
+      <c r="X16" s="9">
+        <v>1.835</v>
+      </c>
+      <c r="Y16" s="19">
+        <v>1.835</v>
+      </c>
+      <c r="Z16" s="19">
+        <v>1.835</v>
+      </c>
+      <c r="AA16" s="19">
+        <v>1.835</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>1.835</v>
+      </c>
+      <c r="AC16" s="5">
         <f t="shared" ref="AC16:AC23" si="9">AVERAGE(X16:AB16)</f>
-        <v>#DIV/0!</v>
+        <v>1.8350000000000002</v>
       </c>
       <c r="AD16" s="9">
         <v>2.6909999999999998</v>
@@ -1787,17 +1981,25 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
+      <c r="D17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H17" s="5" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -1805,10 +2007,18 @@
       <c r="I17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="11"/>
+      <c r="J17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N17" s="5" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
@@ -1823,7 +2033,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U17" s="15"/>
-      <c r="V17" s="19"/>
+      <c r="V17" s="21"/>
       <c r="W17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1876,17 +2086,25 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
+      <c r="D18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H18" s="5" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -1894,10 +2112,18 @@
       <c r="I18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="11"/>
+      <c r="J18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N18" s="5" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
@@ -1912,7 +2138,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U18" s="15"/>
-      <c r="V18" s="19"/>
+      <c r="V18" s="21"/>
       <c r="W18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1965,17 +2191,25 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
+      <c r="D19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H19" s="5" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -1983,10 +2217,18 @@
       <c r="I19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="11"/>
+      <c r="J19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N19" s="5" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
@@ -2001,7 +2243,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U19" s="15"/>
-      <c r="V19" s="19"/>
+      <c r="V19" s="21"/>
       <c r="W19" s="4" t="s">
         <v>5</v>
       </c>
@@ -2054,13 +2296,28 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="5" t="e">
+      <c r="C20">
+        <v>1.724</v>
+      </c>
+      <c r="D20">
+        <v>1.7270000000000001</v>
+      </c>
+      <c r="E20">
+        <v>1.726</v>
+      </c>
+      <c r="F20">
+        <v>1.6850000000000001</v>
+      </c>
+      <c r="G20">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="H20" s="5">
         <f>AVERAGE(C20:G20)</f>
-        <v>#DIV/0!</v>
+        <v>1.7138000000000002</v>
       </c>
       <c r="I20" s="9">
         <v>1.288</v>
@@ -2071,7 +2328,7 @@
       <c r="K20" s="10">
         <v>1.2430000000000001</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="19">
         <v>1.234</v>
       </c>
       <c r="M20" s="11">
@@ -2091,18 +2348,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U20" s="15"/>
-      <c r="V20" s="19"/>
+      <c r="V20" s="21"/>
       <c r="W20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="10"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="5" t="e">
+      <c r="X20" s="9">
+        <v>144.9</v>
+      </c>
+      <c r="Y20" s="10">
+        <v>144.6</v>
+      </c>
+      <c r="Z20" s="10">
+        <v>144.69999999999999</v>
+      </c>
+      <c r="AA20" s="19">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="AB20" s="11">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="AC20" s="5">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>145.76</v>
       </c>
       <c r="AD20" s="9">
         <v>193.9</v>
@@ -2113,7 +2380,7 @@
       <c r="AF20" s="10">
         <v>201</v>
       </c>
-      <c r="AG20" s="22">
+      <c r="AG20" s="19">
         <v>202.4</v>
       </c>
       <c r="AH20" s="11">
@@ -2134,18 +2401,28 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="5" t="e">
+      <c r="C21" s="9">
+        <v>1.8109999999999999</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1.788</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1.8080000000000001</v>
+      </c>
+      <c r="F21" s="19">
+        <v>1.8220000000000001</v>
+      </c>
+      <c r="G21" s="11">
+        <v>1.7909999999999999</v>
+      </c>
+      <c r="H21" s="5">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.8039999999999998</v>
       </c>
       <c r="I21" s="9">
         <v>1.42</v>
@@ -2156,7 +2433,7 @@
       <c r="K21" s="10">
         <v>1.319</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="19">
         <v>1.35</v>
       </c>
       <c r="M21" s="11">
@@ -2176,18 +2453,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U21" s="15"/>
-      <c r="V21" s="19"/>
+      <c r="V21" s="21"/>
       <c r="W21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="10"/>
-      <c r="Z21" s="10"/>
-      <c r="AA21" s="10"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="5" t="e">
+      <c r="X21" s="9">
+        <v>275.89999999999998</v>
+      </c>
+      <c r="Y21" s="10">
+        <v>279.39999999999998</v>
+      </c>
+      <c r="Z21" s="10">
+        <v>276.3</v>
+      </c>
+      <c r="AA21" s="19">
+        <v>274.2</v>
+      </c>
+      <c r="AB21" s="11">
+        <v>278.89999999999998</v>
+      </c>
+      <c r="AC21" s="5">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>276.93999999999994</v>
       </c>
       <c r="AD21" s="9">
         <v>351.8</v>
@@ -2198,7 +2485,7 @@
       <c r="AF21" s="10">
         <v>378.7</v>
       </c>
-      <c r="AG21" s="22">
+      <c r="AG21" s="19">
         <v>370.1</v>
       </c>
       <c r="AH21" s="11">
@@ -2219,18 +2506,28 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="5" t="e">
+      <c r="C22" s="9">
+        <v>1.996</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1.8009999999999999</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1.8220000000000001</v>
+      </c>
+      <c r="F22" s="19">
+        <v>1.825</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1.843</v>
+      </c>
+      <c r="H22" s="5">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.8573999999999997</v>
       </c>
       <c r="I22" s="9">
         <v>1.444</v>
@@ -2241,7 +2538,7 @@
       <c r="K22" s="10">
         <v>1.38</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="19">
         <v>1.395</v>
       </c>
       <c r="M22" s="11">
@@ -2261,18 +2558,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="19"/>
+      <c r="V22" s="21"/>
       <c r="W22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="10"/>
-      <c r="AA22" s="10"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="5" t="e">
+      <c r="X22" s="9">
+        <v>375.4</v>
+      </c>
+      <c r="Y22" s="10">
+        <v>416</v>
+      </c>
+      <c r="Z22" s="10">
+        <v>411.2</v>
+      </c>
+      <c r="AA22" s="19">
+        <v>410.6</v>
+      </c>
+      <c r="AB22" s="11">
+        <v>406.5</v>
+      </c>
+      <c r="AC22" s="5">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>403.93999999999994</v>
       </c>
       <c r="AD22" s="9">
         <v>519</v>
@@ -2283,7 +2590,7 @@
       <c r="AF22" s="10">
         <v>542.79999999999995</v>
       </c>
-      <c r="AG22" s="22">
+      <c r="AG22" s="19">
         <v>537.20000000000005</v>
       </c>
       <c r="AH22" s="11">
@@ -2304,18 +2611,28 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="5" t="e">
+      <c r="C23" s="12">
+        <v>1.9239999999999999</v>
+      </c>
+      <c r="D23" s="13">
+        <v>2.133</v>
+      </c>
+      <c r="E23" s="13">
+        <v>2.14</v>
+      </c>
+      <c r="F23" s="13">
+        <v>2.117</v>
+      </c>
+      <c r="G23" s="14">
+        <v>1.974</v>
+      </c>
+      <c r="H23" s="5">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>2.0575999999999999</v>
       </c>
       <c r="I23" s="12">
         <v>1.472</v>
@@ -2346,18 +2663,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U23" s="15"/>
-      <c r="V23" s="19"/>
+      <c r="V23" s="21"/>
       <c r="W23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
-      <c r="AB23" s="14"/>
-      <c r="AC23" s="5" t="e">
+      <c r="X23" s="12">
+        <v>519.20000000000005</v>
+      </c>
+      <c r="Y23" s="13">
+        <v>468.4</v>
+      </c>
+      <c r="Z23" s="13">
+        <v>466.8</v>
+      </c>
+      <c r="AA23" s="13">
+        <v>471.9</v>
+      </c>
+      <c r="AB23" s="14">
+        <v>506.1</v>
+      </c>
+      <c r="AC23" s="5">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>486.48</v>
       </c>
       <c r="AD23" s="12">
         <v>678.5</v>
@@ -2432,20 +2759,30 @@
       <c r="AO24" s="15"/>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="5" t="e">
+      <c r="C25" s="6">
+        <v>11.191000000000001</v>
+      </c>
+      <c r="D25" s="7">
+        <v>11.218</v>
+      </c>
+      <c r="E25" s="7">
+        <v>11.252000000000001</v>
+      </c>
+      <c r="F25" s="7">
+        <v>11.253</v>
+      </c>
+      <c r="G25" s="8">
+        <v>11.256</v>
+      </c>
+      <c r="H25" s="5">
         <f>AVERAGE(C25:G25)</f>
-        <v>#DIV/0!</v>
+        <v>11.234</v>
       </c>
       <c r="I25" s="6">
         <v>8.2040000000000006</v>
@@ -2476,20 +2813,30 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U25" s="15"/>
-      <c r="V25" s="19" t="s">
+      <c r="V25" s="21" t="s">
         <v>21</v>
       </c>
       <c r="W25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="7"/>
-      <c r="Z25" s="7"/>
-      <c r="AA25" s="7"/>
-      <c r="AB25" s="8"/>
-      <c r="AC25" s="5" t="e">
+      <c r="X25" s="6">
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="Y25" s="7">
+        <v>2.6480000000000001</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>2.64</v>
+      </c>
+      <c r="AA25" s="7">
+        <v>2.64</v>
+      </c>
+      <c r="AB25" s="8">
+        <v>2.6389999999999998</v>
+      </c>
+      <c r="AC25" s="5">
         <f>AVERAGE(X25:AB25)</f>
-        <v>#DIV/0!</v>
+        <v>2.6442000000000001</v>
       </c>
       <c r="AD25" s="6">
         <v>3.621</v>
@@ -2521,20 +2868,28 @@
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="9">
         <v>2645.5079999999998</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
+      <c r="D26" s="19">
+        <v>2645.8910000000001</v>
+      </c>
+      <c r="E26" s="19">
+        <v>2645.94</v>
+      </c>
+      <c r="F26" s="19">
+        <v>2646.2370000000001</v>
+      </c>
+      <c r="G26" s="11">
+        <v>2646.183</v>
+      </c>
       <c r="H26" s="5">
         <f t="shared" ref="H26:H33" si="12">AVERAGE(C26:G26)</f>
-        <v>2645.5079999999998</v>
+        <v>2645.9518000000003</v>
       </c>
       <c r="I26" s="9">
         <v>1692.23</v>
@@ -2557,20 +2912,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U26" s="15"/>
-      <c r="V26" s="19"/>
+      <c r="V26" s="21"/>
       <c r="W26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="X26" s="9">
         <v>2.2229999999999999</v>
       </c>
-      <c r="Y26" s="10"/>
-      <c r="Z26" s="10"/>
-      <c r="AA26" s="10"/>
-      <c r="AB26" s="11"/>
+      <c r="Y26" s="19">
+        <v>2.2229999999999999</v>
+      </c>
+      <c r="Z26" s="19">
+        <v>2.222</v>
+      </c>
+      <c r="AA26" s="19">
+        <v>2.222</v>
+      </c>
+      <c r="AB26" s="11">
+        <v>2.222</v>
+      </c>
       <c r="AC26" s="5">
         <f t="shared" ref="AC26:AC33" si="15">AVERAGE(X26:AB26)</f>
-        <v>2.2229999999999999</v>
+        <v>2.2223999999999995</v>
       </c>
       <c r="AD26" s="9">
         <v>3.4750000000000001</v>
@@ -2594,17 +2957,25 @@
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
+      <c r="D27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H27" s="5" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -2612,10 +2983,18 @@
       <c r="I27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="11"/>
+      <c r="J27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N27" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
@@ -2630,7 +3009,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U27" s="15"/>
-      <c r="V27" s="19"/>
+      <c r="V27" s="21"/>
       <c r="W27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2683,17 +3062,25 @@
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="11"/>
+      <c r="D28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H28" s="5" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -2701,10 +3088,18 @@
       <c r="I28" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="11"/>
+      <c r="J28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N28" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
@@ -2719,7 +3114,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U28" s="15"/>
-      <c r="V28" s="19"/>
+      <c r="V28" s="21"/>
       <c r="W28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2772,17 +3167,25 @@
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="11"/>
+      <c r="D29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H29" s="5" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -2790,10 +3193,18 @@
       <c r="I29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="11"/>
+      <c r="J29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N29" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
@@ -2808,7 +3219,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U29" s="15"/>
-      <c r="V29" s="19"/>
+      <c r="V29" s="21"/>
       <c r="W29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2861,18 +3272,28 @@
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="5" t="e">
+      <c r="C30" s="9">
+        <v>1.625</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1.603</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1.6040000000000001</v>
+      </c>
+      <c r="F30" s="19">
+        <v>1.651</v>
+      </c>
+      <c r="G30" s="11">
+        <v>1.6579999999999999</v>
+      </c>
+      <c r="H30" s="5">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1.6282000000000001</v>
       </c>
       <c r="I30" s="9">
         <v>1.069</v>
@@ -2883,7 +3304,7 @@
       <c r="K30" s="10">
         <v>1.0149999999999999</v>
       </c>
-      <c r="L30" s="22">
+      <c r="L30" s="19">
         <v>1</v>
       </c>
       <c r="M30" s="11">
@@ -2903,18 +3324,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U30" s="15"/>
-      <c r="V30" s="19"/>
+      <c r="V30" s="21"/>
       <c r="W30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X30" s="9"/>
-      <c r="Y30" s="10"/>
-      <c r="Z30" s="10"/>
-      <c r="AA30" s="10"/>
-      <c r="AB30" s="11"/>
-      <c r="AC30" s="5" t="e">
+      <c r="X30" s="9">
+        <v>153.69999999999999</v>
+      </c>
+      <c r="Y30" s="10">
+        <v>155.80000000000001</v>
+      </c>
+      <c r="Z30" s="10">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="AA30" s="19">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="AB30" s="11">
+        <v>150.69999999999999</v>
+      </c>
+      <c r="AC30" s="5">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+        <v>153.44</v>
       </c>
       <c r="AD30" s="9">
         <v>233.7</v>
@@ -2925,7 +3356,7 @@
       <c r="AF30" s="10">
         <v>246.1</v>
       </c>
-      <c r="AG30" s="22">
+      <c r="AG30" s="19">
         <v>249.8</v>
       </c>
       <c r="AH30" s="11">
@@ -2946,18 +3377,28 @@
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="5" t="e">
+      <c r="C31" s="9">
+        <v>1.647</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1.6279999999999999</v>
+      </c>
+      <c r="E31" s="10">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="F31" s="19">
+        <v>1.629</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1.653</v>
+      </c>
+      <c r="H31" s="5">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1.6362000000000001</v>
       </c>
       <c r="I31" s="9">
         <v>1.3640000000000001</v>
@@ -2968,7 +3409,7 @@
       <c r="K31" s="10">
         <v>1.3089999999999999</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="19">
         <v>1.06</v>
       </c>
       <c r="M31" s="11">
@@ -2988,18 +3429,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U31" s="15"/>
-      <c r="V31" s="19"/>
+      <c r="V31" s="21"/>
       <c r="W31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="10"/>
-      <c r="Z31" s="10"/>
-      <c r="AA31" s="10"/>
-      <c r="AB31" s="11"/>
-      <c r="AC31" s="5" t="e">
+      <c r="X31" s="9">
+        <v>303.3</v>
+      </c>
+      <c r="Y31" s="10">
+        <v>306.89999999999998</v>
+      </c>
+      <c r="Z31" s="10">
+        <v>307.60000000000002</v>
+      </c>
+      <c r="AA31" s="19">
+        <v>306.7</v>
+      </c>
+      <c r="AB31" s="11">
+        <v>302.2</v>
+      </c>
+      <c r="AC31" s="5">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+        <v>305.34000000000003</v>
       </c>
       <c r="AD31" s="9">
         <v>366.2</v>
@@ -3010,7 +3461,7 @@
       <c r="AF31" s="10">
         <v>381.7</v>
       </c>
-      <c r="AG31" s="22">
+      <c r="AG31" s="19">
         <v>382.6</v>
       </c>
       <c r="AH31" s="11">
@@ -3031,18 +3482,28 @@
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="5" t="e">
+      <c r="C32" s="9">
+        <v>1.6879999999999999</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1.659</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1.659</v>
+      </c>
+      <c r="F32" s="19">
+        <v>1.66</v>
+      </c>
+      <c r="G32" s="11">
+        <v>1.671</v>
+      </c>
+      <c r="H32" s="5">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1.6674</v>
       </c>
       <c r="I32" s="9">
         <v>1.401</v>
@@ -3053,7 +3514,7 @@
       <c r="K32" s="10">
         <v>1.3280000000000001</v>
       </c>
-      <c r="L32" s="22">
+      <c r="L32" s="19">
         <v>1.3169999999999999</v>
       </c>
       <c r="M32" s="11">
@@ -3073,18 +3534,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U32" s="15"/>
-      <c r="V32" s="19"/>
+      <c r="V32" s="21"/>
       <c r="W32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="10"/>
-      <c r="Z32" s="10"/>
-      <c r="AA32" s="10"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="5" t="e">
+      <c r="X32" s="9">
+        <v>443.9</v>
+      </c>
+      <c r="Y32" s="10">
+        <v>451.6</v>
+      </c>
+      <c r="Z32" s="10">
+        <v>451.6</v>
+      </c>
+      <c r="AA32" s="19">
+        <v>451.4</v>
+      </c>
+      <c r="AB32" s="11">
+        <v>448.4</v>
+      </c>
+      <c r="AC32" s="5">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+        <v>449.38</v>
       </c>
       <c r="AD32" s="9">
         <v>535</v>
@@ -3095,7 +3566,7 @@
       <c r="AF32" s="10">
         <v>564.4</v>
       </c>
-      <c r="AG32" s="22">
+      <c r="AG32" s="19">
         <v>569</v>
       </c>
       <c r="AH32" s="11">
@@ -3116,18 +3587,28 @@
       </c>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="5" t="e">
+      <c r="C33" s="12">
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1.9039999999999999</v>
+      </c>
+      <c r="E33" s="13">
+        <v>1.91</v>
+      </c>
+      <c r="F33" s="13">
+        <v>1.732</v>
+      </c>
+      <c r="G33" s="14">
+        <v>1.7310000000000001</v>
+      </c>
+      <c r="H33" s="5">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1.802</v>
       </c>
       <c r="I33" s="12">
         <v>1.413</v>
@@ -3158,18 +3639,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U33" s="15"/>
-      <c r="V33" s="19"/>
+      <c r="V33" s="21"/>
       <c r="W33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X33" s="12"/>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="13"/>
-      <c r="AB33" s="14"/>
-      <c r="AC33" s="5" t="e">
+      <c r="X33" s="12">
+        <v>576.5</v>
+      </c>
+      <c r="Y33" s="13">
+        <v>524.70000000000005</v>
+      </c>
+      <c r="Z33" s="13">
+        <v>523</v>
+      </c>
+      <c r="AA33" s="13">
+        <v>576.79999999999995</v>
+      </c>
+      <c r="AB33" s="14">
+        <v>577.1</v>
+      </c>
+      <c r="AC33" s="5">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+        <v>555.62</v>
       </c>
       <c r="AD33" s="12">
         <v>707.2</v>
@@ -3244,20 +3735,30 @@
       <c r="AO34" s="15"/>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="5" t="e">
+      <c r="C35" s="6">
+        <v>10.314</v>
+      </c>
+      <c r="D35" s="7">
+        <v>10.355</v>
+      </c>
+      <c r="E35" s="7">
+        <v>10.298</v>
+      </c>
+      <c r="F35" s="7">
+        <v>10.368</v>
+      </c>
+      <c r="G35" s="8">
+        <v>10.366</v>
+      </c>
+      <c r="H35" s="5">
         <f>AVERAGE(C35:G35)</f>
-        <v>#DIV/0!</v>
+        <v>10.340199999999999</v>
       </c>
       <c r="I35" s="6">
         <v>7.6390000000000002</v>
@@ -3288,20 +3789,30 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U35" s="15"/>
-      <c r="V35" s="19" t="s">
+      <c r="V35" s="21" t="s">
         <v>22</v>
       </c>
       <c r="W35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="7"/>
-      <c r="Z35" s="7"/>
-      <c r="AA35" s="7"/>
-      <c r="AB35" s="8"/>
-      <c r="AC35" s="5" t="e">
+      <c r="X35" s="6">
+        <v>2.88</v>
+      </c>
+      <c r="Y35" s="7">
+        <v>2.8690000000000002</v>
+      </c>
+      <c r="Z35" s="7">
+        <v>2.8839999999999999</v>
+      </c>
+      <c r="AA35" s="7">
+        <v>2.8650000000000002</v>
+      </c>
+      <c r="AB35" s="8">
+        <v>2.8660000000000001</v>
+      </c>
+      <c r="AC35" s="5">
         <f>AVERAGE(X35:AB35)</f>
-        <v>#DIV/0!</v>
+        <v>2.8728000000000002</v>
       </c>
       <c r="AD35" s="6">
         <v>3.8889999999999998</v>
@@ -3333,7 +3844,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
@@ -3351,13 +3862,15 @@
       <c r="I36" s="9">
         <v>1584.7449999999999</v>
       </c>
-      <c r="J36" s="10"/>
+      <c r="J36" s="19">
+        <v>1584.5709999999999</v>
+      </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="11"/>
       <c r="N36" s="5">
         <f t="shared" ref="N36:N43" si="19">AVERAGE(I36:M36)</f>
-        <v>1584.7449999999999</v>
+        <v>1584.6579999999999</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="10"/>
@@ -3369,7 +3882,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U36" s="15"/>
-      <c r="V36" s="19"/>
+      <c r="V36" s="21"/>
       <c r="W36" s="4" t="s">
         <v>2</v>
       </c>
@@ -3387,7 +3900,9 @@
       <c r="AD36" s="9">
         <v>3.7109999999999999</v>
       </c>
-      <c r="AE36" s="10"/>
+      <c r="AE36" s="19">
+        <v>3.7109999999999999</v>
+      </c>
       <c r="AF36" s="10"/>
       <c r="AG36" s="10"/>
       <c r="AH36" s="11"/>
@@ -3406,17 +3921,25 @@
       </c>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="11"/>
+      <c r="D37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H37" s="5" t="e">
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
@@ -3424,10 +3947,18 @@
       <c r="I37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="11"/>
+      <c r="J37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N37" s="5" t="e">
         <f t="shared" si="19"/>
         <v>#DIV/0!</v>
@@ -3442,7 +3973,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U37" s="15"/>
-      <c r="V37" s="19"/>
+      <c r="V37" s="21"/>
       <c r="W37" s="4" t="s">
         <v>3</v>
       </c>
@@ -3495,17 +4026,25 @@
       </c>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="11"/>
+      <c r="D38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H38" s="5" t="e">
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
@@ -3513,10 +4052,18 @@
       <c r="I38" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="11"/>
+      <c r="J38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N38" s="5" t="e">
         <f t="shared" si="19"/>
         <v>#DIV/0!</v>
@@ -3531,7 +4078,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U38" s="15"/>
-      <c r="V38" s="19"/>
+      <c r="V38" s="21"/>
       <c r="W38" s="4" t="s">
         <v>4</v>
       </c>
@@ -3584,17 +4131,25 @@
       </c>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="11"/>
+      <c r="D39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H39" s="5" t="e">
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
@@ -3602,10 +4157,18 @@
       <c r="I39" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="11"/>
+      <c r="J39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N39" s="5" t="e">
         <f t="shared" si="19"/>
         <v>#DIV/0!</v>
@@ -3620,7 +4183,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U39" s="15"/>
-      <c r="V39" s="19"/>
+      <c r="V39" s="21"/>
       <c r="W39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3673,18 +4236,28 @@
       </c>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="5" t="e">
+      <c r="C40" s="9">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="D40" s="10">
+        <v>1.49</v>
+      </c>
+      <c r="E40" s="10">
+        <v>1.494</v>
+      </c>
+      <c r="F40" s="19">
+        <v>1.486</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1.4870000000000001</v>
+      </c>
+      <c r="H40" s="5">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.4936</v>
       </c>
       <c r="I40" s="9">
         <v>1.0289999999999999</v>
@@ -3695,7 +4268,7 @@
       <c r="K40" s="10">
         <v>0.93799999999999994</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="19">
         <v>0.93799999999999994</v>
       </c>
       <c r="M40" s="11">
@@ -3715,18 +4288,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U40" s="15"/>
-      <c r="V40" s="19"/>
+      <c r="V40" s="21"/>
       <c r="W40" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X40" s="9"/>
-      <c r="Y40" s="10"/>
-      <c r="Z40" s="10"/>
-      <c r="AA40" s="10"/>
-      <c r="AB40" s="11"/>
-      <c r="AC40" s="5" t="e">
+      <c r="X40" s="9">
+        <v>165.3</v>
+      </c>
+      <c r="Y40" s="10">
+        <v>167.7</v>
+      </c>
+      <c r="Z40" s="10">
+        <v>167.2</v>
+      </c>
+      <c r="AA40" s="19">
+        <v>168.1</v>
+      </c>
+      <c r="AB40" s="11">
+        <v>168</v>
+      </c>
+      <c r="AC40" s="5">
         <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
+        <v>167.26</v>
       </c>
       <c r="AD40" s="9">
         <v>242.8</v>
@@ -3737,7 +4320,7 @@
       <c r="AF40" s="10">
         <v>266.39999999999998</v>
       </c>
-      <c r="AG40" s="22">
+      <c r="AG40" s="19">
         <v>266.3</v>
       </c>
       <c r="AH40" s="11">
@@ -3758,18 +4341,28 @@
       </c>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="5" t="e">
+      <c r="C41" s="9">
+        <v>1.5880000000000001</v>
+      </c>
+      <c r="D41" s="10">
+        <v>1.579</v>
+      </c>
+      <c r="E41" s="10">
+        <v>1.5840000000000001</v>
+      </c>
+      <c r="F41" s="19">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="G41" s="11">
+        <v>1.5649999999999999</v>
+      </c>
+      <c r="H41" s="5">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.5767999999999998</v>
       </c>
       <c r="I41" s="9">
         <v>1.2969999999999999</v>
@@ -3780,7 +4373,7 @@
       <c r="K41" s="10">
         <v>1.2310000000000001</v>
       </c>
-      <c r="L41" s="22">
+      <c r="L41" s="19">
         <v>1.232</v>
       </c>
       <c r="M41" s="11">
@@ -3800,18 +4393,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U41" s="15"/>
-      <c r="V41" s="19"/>
+      <c r="V41" s="21"/>
       <c r="W41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X41" s="9"/>
-      <c r="Y41" s="10"/>
-      <c r="Z41" s="10"/>
-      <c r="AA41" s="10"/>
-      <c r="AB41" s="11"/>
-      <c r="AC41" s="5" t="e">
+      <c r="X41" s="9">
+        <v>314.60000000000002</v>
+      </c>
+      <c r="Y41" s="10">
+        <v>316.39999999999998</v>
+      </c>
+      <c r="Z41" s="10">
+        <v>315.39999999999998</v>
+      </c>
+      <c r="AA41" s="19">
+        <v>318.60000000000002</v>
+      </c>
+      <c r="AB41" s="11">
+        <v>319.2</v>
+      </c>
+      <c r="AC41" s="5">
         <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
+        <v>316.84000000000003</v>
       </c>
       <c r="AD41" s="9">
         <v>385</v>
@@ -3822,7 +4425,7 @@
       <c r="AF41" s="10">
         <v>405.7</v>
       </c>
-      <c r="AG41" s="22">
+      <c r="AG41" s="19">
         <v>405.6</v>
       </c>
       <c r="AH41" s="11">
@@ -3843,18 +4446,28 @@
       </c>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="5" t="e">
+      <c r="C42" s="9">
+        <v>1.601</v>
+      </c>
+      <c r="D42" s="10">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="E42" s="10">
+        <v>1.597</v>
+      </c>
+      <c r="F42" s="19">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="G42" s="11">
+        <v>1.605</v>
+      </c>
+      <c r="H42" s="5">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.6046</v>
       </c>
       <c r="I42" s="9">
         <v>1.2969999999999999</v>
@@ -3865,7 +4478,7 @@
       <c r="K42" s="10">
         <v>1.2669999999999999</v>
       </c>
-      <c r="L42" s="22">
+      <c r="L42" s="19">
         <v>1.2669999999999999</v>
       </c>
       <c r="M42" s="11">
@@ -3885,18 +4498,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U42" s="15"/>
-      <c r="V42" s="19"/>
+      <c r="V42" s="21"/>
       <c r="W42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="X42" s="9"/>
-      <c r="Y42" s="10"/>
-      <c r="Z42" s="10"/>
-      <c r="AA42" s="10"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="5" t="e">
+      <c r="X42" s="9">
+        <v>468</v>
+      </c>
+      <c r="Y42" s="10">
+        <v>466</v>
+      </c>
+      <c r="Z42" s="10">
+        <v>469.2</v>
+      </c>
+      <c r="AA42" s="19">
+        <v>464.8</v>
+      </c>
+      <c r="AB42" s="11">
+        <v>466.8</v>
+      </c>
+      <c r="AC42" s="5">
         <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
+        <v>466.96000000000004</v>
       </c>
       <c r="AD42" s="9">
         <v>577.79999999999995</v>
@@ -3907,7 +4530,7 @@
       <c r="AF42" s="10">
         <v>591.6</v>
       </c>
-      <c r="AG42" s="22">
+      <c r="AG42" s="19">
         <v>591.29999999999995</v>
       </c>
       <c r="AH42" s="11">
@@ -3928,18 +4551,28 @@
       </c>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="5" t="e">
+      <c r="C43" s="12">
+        <v>1.732</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1.7589999999999999</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="F43" s="13">
+        <v>1.67</v>
+      </c>
+      <c r="G43" s="14">
+        <v>1.925</v>
+      </c>
+      <c r="H43" s="5">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.7504000000000002</v>
       </c>
       <c r="I43" s="12">
         <v>1.36</v>
@@ -3970,18 +4603,28 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U43" s="15"/>
-      <c r="V43" s="19"/>
+      <c r="V43" s="21"/>
       <c r="W43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="13"/>
-      <c r="Z43" s="13"/>
-      <c r="AA43" s="13"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="5" t="e">
+      <c r="X43" s="12">
+        <v>576.79999999999995</v>
+      </c>
+      <c r="Y43" s="13">
+        <v>567.9</v>
+      </c>
+      <c r="Z43" s="13">
+        <v>599.6</v>
+      </c>
+      <c r="AA43" s="13">
+        <v>598.20000000000005</v>
+      </c>
+      <c r="AB43" s="14">
+        <v>519</v>
+      </c>
+      <c r="AC43" s="5">
         <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
+        <v>572.29999999999995</v>
       </c>
       <c r="AD43" s="12">
         <v>734.5</v>
@@ -4179,6 +4822,7 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:N3"/>
     <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="V1:X2"/>
     <mergeCell ref="AJ3:AO3"/>
     <mergeCell ref="V5:V13"/>
     <mergeCell ref="A25:A33"/>
@@ -4188,7 +4832,6 @@
     <mergeCell ref="V15:V23"/>
     <mergeCell ref="V25:V33"/>
     <mergeCell ref="V35:V43"/>
-    <mergeCell ref="V1:X2"/>
     <mergeCell ref="X3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>